<commit_message>
Import devices from excel 2
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>serial_number</t>
   </si>
@@ -68,9 +68,6 @@
     <t>a4</t>
   </si>
   <si>
-    <t>a5</t>
-  </si>
-  <si>
     <t>a6</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>b4</t>
   </si>
   <si>
-    <t>b5</t>
-  </si>
-  <si>
     <t>b6</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>c4</t>
   </si>
   <si>
-    <t>c5</t>
-  </si>
-  <si>
     <t>c6</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
   </si>
   <si>
     <t>e4</t>
-  </si>
-  <si>
-    <t>e5</t>
   </si>
   <si>
     <t>e6</t>
@@ -308,7 +296,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -379,157 +367,157 @@
       <c r="E2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="F4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="I5" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="F6" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="I6" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="J6" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="K6" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import and Export Services
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>serial_number</t>
   </si>
@@ -56,7 +56,7 @@
     <t>aaa-12345</t>
   </si>
   <si>
-    <t>a1</t>
+    <t>a2</t>
   </si>
   <si>
     <t>b1</t>
@@ -92,6 +92,9 @@
     <t>Abcd-2222</t>
   </si>
   <si>
+    <t>c2</t>
+  </si>
+  <si>
     <t>b2</t>
   </si>
   <si>
@@ -122,9 +125,6 @@
     <t>Abcd-3333</t>
   </si>
   <si>
-    <t>c1</t>
-  </si>
-  <si>
     <t>c4</t>
   </si>
   <si>
@@ -149,9 +149,6 @@
     <t>Abcd-4444</t>
   </si>
   <si>
-    <t>d1</t>
-  </si>
-  <si>
     <t>d2</t>
   </si>
   <si>
@@ -173,7 +170,7 @@
     <t>d9</t>
   </si>
   <si>
-    <t>e1</t>
+    <t>abcdefg</t>
   </si>
   <si>
     <t>e2</t>
@@ -296,7 +293,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -397,45 +394,45 @@
         <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>20</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>36</v>
@@ -470,51 +467,54 @@
         <v>44</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="I5" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="B6" s="0" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>40</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="J6" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Added Domain Supervisor (2)
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>serial_number</t>
   </si>
@@ -23,6 +23,9 @@
     <t>device_name</t>
   </si>
   <si>
+    <t>pool_id</t>
+  </si>
+  <si>
     <t>manufacturer</t>
   </si>
   <si>
@@ -59,16 +62,16 @@
     <t>a2</t>
   </si>
   <si>
+    <t>co_hallo_7949</t>
+  </si>
+  <si>
     <t>b1</t>
   </si>
   <si>
     <t>a3</t>
   </si>
   <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>a6</t>
+    <t>hallo@hallo.at, hallo1@hallo.at</t>
   </si>
   <si>
     <t>a7</t>
@@ -83,7 +86,7 @@
     <t>good</t>
   </si>
   <si>
-    <t>asdfkasjdflasjdfkjsadlökfjkölsadjfk asdfhaskdhf jasdhfjk hsadjfhlaskdf</t>
+    <t>aa</t>
   </si>
   <si>
     <t>sadf</t>
@@ -101,10 +104,7 @@
     <t>b3</t>
   </si>
   <si>
-    <t>b4</t>
-  </si>
-  <si>
-    <t>b6</t>
+    <t>hallo@hallo.at, hallo2@hallo.at</t>
   </si>
   <si>
     <t>b7</t>
@@ -119,13 +119,16 @@
     <t>best</t>
   </si>
   <si>
+    <t>bb</t>
+  </si>
+  <si>
     <t>asf</t>
   </si>
   <si>
     <t>Abcd-3333</t>
   </si>
   <si>
-    <t>c4</t>
+    <t>co_hallo1_9778</t>
   </si>
   <si>
     <t>c6</t>
@@ -143,6 +146,9 @@
     <t>ok</t>
   </si>
   <si>
+    <t>cc</t>
+  </si>
+  <si>
     <t>asdf</t>
   </si>
   <si>
@@ -155,9 +161,6 @@
     <t>d3</t>
   </si>
   <si>
-    <t>d4</t>
-  </si>
-  <si>
     <t>d6</t>
   </si>
   <si>
@@ -170,6 +173,9 @@
     <t>d9</t>
   </si>
   <si>
+    <t>dd</t>
+  </si>
+  <si>
     <t>abcdefg</t>
   </si>
   <si>
@@ -179,9 +185,6 @@
     <t>e3</t>
   </si>
   <si>
-    <t>e4</t>
-  </si>
-  <si>
     <t>e6</t>
   </si>
   <si>
@@ -189,6 +192,9 @@
   </si>
   <si>
     <t>e9</t>
+  </si>
+  <si>
+    <t>ee</t>
   </si>
 </sst>
 </file>
@@ -293,16 +299,14 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.4412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1133603238866"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5546558704453"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.1133603238866"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.5748987854251"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4412955465587"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5748987854251"/>
   </cols>
@@ -321,83 +325,83 @@
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>27</v>
@@ -423,101 +427,110 @@
       <c r="K3" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="L3" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="M3" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>30</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>40</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formated detailed description | enabled html with sanitization
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -617,7 +617,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
   <si>
     <t>Model</t>
   </si>
@@ -635,12 +635,6 @@
   </si>
   <si>
     <t>Signal generators</t>
-  </si>
-  <si>
-    <t>Signal analysers</t>
-  </si>
-  <si>
-    <t>Network &amp; Spectrum analysers</t>
   </si>
   <si>
     <t>Oscilloscopes</t>
@@ -866,6 +860,15 @@
     <t>** High current amplitudes for 5 A relay testing
 ** High accuracy and versatility for testing static and numerical relays of all types
 ** Integrated network for testing IEC 61850 IEDs</t>
+  </si>
+  <si>
+    <t>Signal analyzers</t>
+  </si>
+  <si>
+    <t>Signal analzsers</t>
+  </si>
+  <si>
+    <t>Network &amp; Spectrum analyzers</t>
   </si>
 </sst>
 </file>
@@ -1108,15 +1111,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1160,6 +1154,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1625,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1654,148 +1657,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="29" t="s">
+      <c r="L1" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="29" t="s">
+      <c r="W1" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="13" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="30" t="s">
+      <c r="J2" s="29">
+        <v>15000</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="T1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="X1" s="27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" s="13" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="32">
-        <v>15000</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="32" t="s">
+      <c r="R2" s="29">
+        <v>2014</v>
+      </c>
+      <c r="S2" s="29">
+        <v>45600</v>
+      </c>
+      <c r="T2" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q2" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="R2" s="32">
-        <v>2014</v>
-      </c>
-      <c r="S2" s="32">
-        <v>45600</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="32">
+      <c r="U2" s="29">
         <v>450</v>
       </c>
-      <c r="V2" s="32">
+      <c r="V2" s="29">
         <v>150</v>
       </c>
-      <c r="W2" s="32">
+      <c r="W2" s="29">
         <v>390</v>
       </c>
-      <c r="X2" s="34">
+      <c r="X2" s="31">
         <v>16.8</v>
       </c>
     </row>
@@ -3385,7 +3388,7 @@
   <dimension ref="B1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3401,11 +3404,11 @@
         <v>3</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3413,167 +3416,167 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="33"/>
+      <c r="C5" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="33"/>
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
-      <c r="C5" s="3" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="33"/>
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
-      <c r="C6" s="3" t="s">
+    <row r="8" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="34"/>
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="15"/>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
-      <c r="C8" s="4" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="33"/>
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="33"/>
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="15"/>
-      <c r="C10" s="3" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="33"/>
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="3" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="33"/>
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="3" t="s">
+    <row r="14" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="34"/>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="15"/>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="16"/>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="33"/>
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2" t="s">
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="33"/>
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
-      <c r="C16" s="3" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="33"/>
+      <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
-      <c r="C17" s="3" t="s">
+    <row r="19" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="34"/>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="16"/>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="33"/>
+      <c r="C21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2" t="s">
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="33"/>
+      <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
-      <c r="C21" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="15"/>
-      <c r="C22" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="23" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="16"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
@@ -3601,7 +3604,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3617,217 +3620,217 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>6</v>
+        <v>66</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>7</v>
+        <v>50</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="20" t="s">
-        <v>9</v>
+        <v>68</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="17" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="18"/>
-      <c r="D8" s="22" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="15"/>
+      <c r="D9" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="15"/>
+      <c r="D10" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="18"/>
-      <c r="D9" s="22" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="15"/>
+      <c r="D11" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="18"/>
-      <c r="D10" s="22" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="15"/>
+      <c r="D12" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="18"/>
-      <c r="D11" s="22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="18"/>
-      <c r="D12" s="22" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D13" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="17" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="15"/>
+      <c r="D14" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="15"/>
+      <c r="D15" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="18"/>
-      <c r="D14" s="17" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="15"/>
+      <c r="D16" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="18"/>
-      <c r="D15" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="18"/>
-      <c r="D16" s="17" t="s">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="15"/>
+      <c r="D17" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" s="18"/>
-      <c r="D17" s="24" t="s">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="15"/>
+      <c r="D18" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="15"/>
+      <c r="D19" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C18" s="18"/>
-      <c r="D18" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C19" s="18"/>
-      <c r="D19" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C20" s="18"/>
+      <c r="C20" s="15"/>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C21" s="18"/>
-      <c r="D21" s="26" t="s">
-        <v>71</v>
+      <c r="C21" s="15"/>
+      <c r="D21" s="23" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C23" s="18"/>
+      <c r="C23" s="15"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C24" s="18"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C25" s="18"/>
+      <c r="C25" s="15"/>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C26" s="18"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C27" s="18"/>
+      <c r="C27" s="15"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C28" s="18"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C29" s="18"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C31" s="18"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C32" s="18"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="18"/>
+      <c r="C33" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>